<commit_message>
Been working a lot this morning on presentation and code
will update you
</commit_message>
<xml_diff>
--- a/CFA_data.xlsx
+++ b/CFA_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\datdo\Documents\Bethel\11_FinalProject\Datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bringthejoy/Documents/Final Project/Final-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3456412-9DB1-45B7-86C4-A904C8AC7064}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF74F46-6445-0944-9B74-60D6E0AE5AE6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30855" yWindow="555" windowWidth="22425" windowHeight="14430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -480,13 +480,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,7 +536,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -589,7 +589,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -642,7 +642,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -695,7 +695,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -748,7 +748,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -801,7 +801,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -854,7 +854,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -907,7 +907,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -960,7 +960,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1858,10 +1858,10 @@
         <v>57.659503131117567</v>
       </c>
       <c r="Q26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>

</xml_diff>